<commit_message>
Added code to produce a bad generator based on the edge label partition
</commit_message>
<xml_diff>
--- a/generator/testing_data/averages_gen_check.xlsx
+++ b/generator/testing_data/averages_gen_check.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eduardoaguila/OneDrive - Johns Hopkins/Masters/Genomics/FinalProj/Genomics-Final-Project/generator/testing_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livejohnshopkins-my.sharepoint.com/personal/eaguila6_jh_edu/Documents/Masters/Genomics/Final_Project/Genomics-Final-Project/generator/testing_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4DDBB7BD-4851-0A41-B7E4-BD483C454537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{4DDBB7BD-4851-0A41-B7E4-BD483C454537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4F689EA-83B2-7042-9F14-ABF384A470BA}"/>
   <bookViews>
-    <workbookView xWindow="3140" yWindow="2380" windowWidth="28040" windowHeight="17440" activeTab="1"/>
+    <workbookView xWindow="3140" yWindow="2380" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="averages_gen_check" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="22">
   <si>
     <t xml:space="preserve">5	</t>
   </si>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -3202,7 +3202,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:Z30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3613,125 +3613,167 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C3" sqref="C3:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>20</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" s="1">
         <v>4.766</v>
       </c>
       <c r="C4" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D4" s="1">
+        <v>4.766</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" s="1">
         <v>7.8079999999999998</v>
       </c>
       <c r="C5" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D5" s="1">
+        <v>7.8079999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="1">
         <v>12.233000000000001</v>
       </c>
       <c r="C6" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D6" s="1">
+        <v>12.233000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1">
         <v>17.815000000000001</v>
       </c>
       <c r="C7" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D7" s="1">
+        <v>17.815000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B8" s="1">
         <v>22.376000000000001</v>
       </c>
       <c r="C8" s="2">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D8" s="1">
+        <v>22.376000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1">
         <v>26.228000000000002</v>
       </c>
       <c r="C9" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D9" s="1">
+        <v>26.228000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1">
         <v>29.763000000000002</v>
       </c>
       <c r="C10" s="2">
         <v>35</v>
       </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D10" s="1">
+        <v>29.763000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1">
         <v>32.688000000000002</v>
       </c>
       <c r="C11" s="2">
         <v>40</v>
       </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D11" s="1">
+        <v>32.688000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1">
         <v>35.377000000000002</v>
       </c>
       <c r="C12" s="2">
         <v>45</v>
       </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D12" s="1">
+        <v>35.377000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1">
         <v>37.878999999999998</v>
       </c>
       <c r="C13" s="2">
         <v>50</v>
       </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D13" s="1">
+        <v>37.878999999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B14" s="1">
         <v>40.116999999999997</v>
       </c>
       <c r="C14" s="2">
         <v>55</v>
       </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D14" s="1">
+        <v>40.116999999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1">
         <v>42.326999999999998</v>
       </c>
       <c r="C15" s="2">
         <v>60</v>
       </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D15" s="1">
+        <v>42.326999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1">
         <v>44.22</v>
       </c>
       <c r="C16" s="2">
         <v>65</v>
+      </c>
+      <c r="D16" s="1">
+        <v>44.22</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.2">
@@ -3741,6 +3783,9 @@
       <c r="C17" s="2">
         <v>70</v>
       </c>
+      <c r="D17" s="1">
+        <v>46.054000000000002</v>
+      </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B18" s="1">
@@ -3749,6 +3794,9 @@
       <c r="C18" s="2">
         <v>75</v>
       </c>
+      <c r="D18" s="1">
+        <v>48.021000000000001</v>
+      </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B19" s="1">
@@ -3757,6 +3805,9 @@
       <c r="C19" s="2">
         <v>80</v>
       </c>
+      <c r="D19" s="1">
+        <v>49.720999999999997</v>
+      </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B20" s="1">
@@ -3765,6 +3816,9 @@
       <c r="C20" s="2">
         <v>85</v>
       </c>
+      <c r="D20" s="1">
+        <v>51.423000000000002</v>
+      </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B21" s="1">
@@ -3773,6 +3827,9 @@
       <c r="C21" s="2">
         <v>90</v>
       </c>
+      <c r="D21" s="1">
+        <v>53.143999999999998</v>
+      </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B22" s="1">
@@ -3781,6 +3838,9 @@
       <c r="C22" s="2">
         <v>95</v>
       </c>
+      <c r="D22" s="1">
+        <v>54.914999999999999</v>
+      </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B23" s="1">
@@ -3789,12 +3849,16 @@
       <c r="C23" s="2">
         <v>100</v>
       </c>
+      <c r="D23" s="1">
+        <v>56.633000000000003</v>
+      </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.2">
       <c r="H31" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>